<commit_message>
label updates for circulators
</commit_message>
<xml_diff>
--- a/routes/er-circulator-listings.xlsx
+++ b/routes/er-circulator-listings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sfrees/projects/hi-er/routes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFA13F8-E131-A343-A3EB-A4CB58D45ACB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC973559-6C76-ED48-BFDA-18A6FC38D11B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30900" windowHeight="18980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,9 +386,6 @@
     <t>HI Laboratory Number</t>
   </si>
   <si>
-    <t>I. No Speed Control</t>
-  </si>
-  <si>
     <t>II. Pressure  Control</t>
   </si>
   <si>
@@ -595,6 +592,9 @@
     <t xml:space="preserve">
 Method I.
 Select Yes if pump uses full speed</t>
+  </si>
+  <si>
+    <t>I. Full Speed</t>
   </si>
 </sst>
 </file>
@@ -1136,39 +1136,6 @@
   </cellStyleXfs>
   <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1327,6 +1294,39 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1713,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1753,362 +1753,367 @@
     <col min="39" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="17" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:38" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="10" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="9" t="s">
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9" t="s">
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="9"/>
-      <c r="X1" s="8" t="s">
+      <c r="W1" s="64"/>
+      <c r="X1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="7" t="s">
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="6" t="s">
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="12" t="s">
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="56"/>
+      <c r="AH1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AI1" s="13" t="s">
+      <c r="AI1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AK1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" s="16" t="s">
+      <c r="AL1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="18" t="s">
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="T2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="U2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="W2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="22" t="s">
+      <c r="X2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="23" t="s">
+      <c r="Y2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="Z2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="22" t="s">
+      <c r="AB2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" s="25" t="s">
+      <c r="AC2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AD2" s="26" t="s">
+      <c r="AD2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="27" t="s">
+      <c r="AE2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="AF2" s="27" t="s">
+      <c r="AF2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AG2" s="28" t="s">
+      <c r="AG2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="29" t="s">
+      <c r="AH2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="AI2" s="30" t="s">
+      <c r="AI2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AJ2" s="31" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" s="32" t="s">
+      <c r="AK2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="AL2" s="32" t="s">
+      <c r="AL2" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="J3" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="K3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="L3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="M3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="N3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="O3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="38" t="s">
+      <c r="P3" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="39" t="s">
+      <c r="Q3" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="40" t="s">
+      <c r="R3" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="41" t="s">
+      <c r="S3" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="42" t="s">
+      <c r="T3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="42" t="s">
+      <c r="U3" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="43" t="s">
+      <c r="V3" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="V3" s="44" t="s">
+      <c r="W3" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="W3" s="43" t="s">
+      <c r="X3" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="X3" s="45" t="s">
+      <c r="Y3" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="Y3" s="46" t="s">
+      <c r="Z3" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="46" t="s">
+      <c r="AA3" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="47" t="s">
+      <c r="AB3" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="AB3" s="45" t="s">
+      <c r="AC3" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="AC3" s="48" t="s">
+      <c r="AD3" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="AD3" s="49" t="s">
+      <c r="AE3" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="50" t="s">
+      <c r="AF3" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="50" t="s">
+      <c r="AG3" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="AG3" s="51" t="s">
+      <c r="AH3" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="AH3" s="52" t="s">
+      <c r="AI3" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="AI3" s="53" t="s">
+      <c r="AJ3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="AJ3" s="54" t="s">
+      <c r="AK3" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="55" t="s">
+      <c r="AL3" s="44" t="s">
         <v>61</v>
-      </c>
-      <c r="AL3" s="55" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:38" ht="245.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="D4" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="57" t="s">
+      <c r="F4" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="G4" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="H4" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="I4" s="60" t="s">
+      <c r="J4" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="K4" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="K4" s="60" t="s">
+      <c r="L4" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="60" t="s">
+      <c r="M4" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="M4" s="60" t="s">
+      <c r="N4" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="O4" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="P4" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="N4" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="O4" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="P4" s="61" t="s">
+      <c r="Q4" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="Q4" s="62" t="s">
+      <c r="R4" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="4" t="s">
+      <c r="W4" s="58"/>
+      <c r="X4" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="W4" s="4"/>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="2" t="s">
+      <c r="AC4" s="60"/>
+      <c r="AD4" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="61"/>
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="61"/>
+      <c r="AH4" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI4" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ4" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI4" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ4" s="64" t="s">
+      <c r="AK4" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="AK4" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL4" s="65" t="s">
-        <v>81</v>
+      <c r="AL4" s="54" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:Q2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="R4:U4"/>
@@ -2116,11 +2121,6 @@
     <mergeCell ref="X4:AA4"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:Q2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2144,44 +2144,44 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
         <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change all Most/Least Consumptive -> Least/Most Efficient
</commit_message>
<xml_diff>
--- a/routes/er-circulator-listings.xlsx
+++ b/routes/er-circulator-listings.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esuarez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hi-er\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E498C4B3-70EF-44FB-A4F7-C23F8BE79FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13395" windowHeight="5190" tabRatio="500"/>
+    <workbookView xWindow="5448" yWindow="3624" windowWidth="23040" windowHeight="12168" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -33,30 +29,12 @@
     <t>Control Methods</t>
   </si>
   <si>
-    <t>Rated (Least Consumptive) Driver or Control Input Power</t>
-  </si>
-  <si>
-    <t>Rated (Least consumptive) Weighted Average Input Power</t>
-  </si>
-  <si>
-    <t>Most Consumptive Driver or Control Input Power</t>
-  </si>
-  <si>
-    <t>Most Consumptive Weighted Average Input Power</t>
-  </si>
-  <si>
     <t xml:space="preserve">Head </t>
   </si>
   <si>
     <t>Flow Rate</t>
   </si>
   <si>
-    <t>Least Consumptive ER</t>
-  </si>
-  <si>
-    <t>Most Consumptive ER</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="22"/>
@@ -371,54 +349,6 @@
     <t>VI. Manual Speed Control</t>
   </si>
   <si>
-    <t>Rated (Least Consumptive) Control Method</t>
-  </si>
-  <si>
-    <t>Most Consumptive Control Method</t>
-  </si>
-  <si>
-    <t>Rated (Least Consumptive) Pressure Curve</t>
-  </si>
-  <si>
-    <t>Most Consumptive Pressure Curve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power  at 25% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power at 50% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point driver or control  input power at 75% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power at 100% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point weigted average input power at maximum rotating speed </t>
-  </si>
-  <si>
-    <t>Rated (Least consumptive) load point weighted average input power at reduced speeds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point driver or control input power  at 25% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point driver or control input power at 50% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point driver or control  input power at 75% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point driver or control input power at 100% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point weigted average input power at maximum rotating speed </t>
-  </si>
-  <si>
-    <t>Most consumptive load point weighted average input power at reduced speeds</t>
-  </si>
-  <si>
     <t xml:space="preserve">Load point head at 25% of BEP at max speed </t>
   </si>
   <si>
@@ -432,18 +362,6 @@
   </si>
   <si>
     <t>Load point flow rate at 100% of BEP</t>
-  </si>
-  <si>
-    <t>Least Consumptive Pump Energy Index on nameplate</t>
-  </si>
-  <si>
-    <t>Most Consumptive Pump Energy Index per HI 41.5</t>
-  </si>
-  <si>
-    <t>Rated (Least consumptive) HI Energy Rating</t>
-  </si>
-  <si>
-    <t>Most consumptive HI Energy Rating</t>
   </si>
   <si>
     <t>(Optional) Alternative number that the participant puts on the nameplate that they would like to be searchable in the HI database.</t>
@@ -478,12 +396,6 @@
 Select Yes if pump uses manual speed control </t>
   </si>
   <si>
-    <t>If Pressure speed control is the rated (least consumptive) control method, insert the control curve equation as function of flow rate(x) and head (y). For example y=mx+b or y=ax^2+bx+c, etc.</t>
-  </si>
-  <si>
-    <t>If Pressure speed control is the most consumptive control method, insert the control curve equation as function of flow rate(x) and head(y). For example y=mx+b or y=ax^2+bx+c, etc.</t>
-  </si>
-  <si>
     <t>Input control input power values for only control methods I, II, III, and IV.</t>
   </si>
   <si>
@@ -535,7 +447,99 @@
     <t>Manual Speed Controls</t>
   </si>
   <si>
-    <t>Input the Rated (Least Consumptive) control method used on the pump.
+    <t xml:space="preserve">
+Method I.
+Select Yes if pump uses full speed</t>
+  </si>
+  <si>
+    <t>I. Full Speed</t>
+  </si>
+  <si>
+    <t>CEI</t>
+  </si>
+  <si>
+    <t>Brand name is displayed on the large label</t>
+  </si>
+  <si>
+    <t>Must be clearly listed on the permanently affixed pump nameplate.</t>
+  </si>
+  <si>
+    <t>Rated (Most efficient) Driver or Control Input Power</t>
+  </si>
+  <si>
+    <t>Rated (Most efficient) Weighted Average Input Power</t>
+  </si>
+  <si>
+    <t>Least Efficient Driver or Control Input Power</t>
+  </si>
+  <si>
+    <t>Least Efficient Weighted Average Input Power</t>
+  </si>
+  <si>
+    <t>Version 1.4</t>
+  </si>
+  <si>
+    <t>Rated (Most Efficient) Control Method</t>
+  </si>
+  <si>
+    <t>Least Efficient Control Method</t>
+  </si>
+  <si>
+    <t>Rated (Most Efficient) Pressure Curve</t>
+  </si>
+  <si>
+    <t>Least Efficient Pressure Curve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Most efficient) load point driver or control input power  at 25% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Most efficient) load point driver or control input power at 50% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Most efficient) load point driver or control  input power at 75% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Most efficient) load point driver or control input power at 100% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Most efficient) load point weigted average input power at maximum rotating speed </t>
+  </si>
+  <si>
+    <t>Rated (Most efficient) load point weighted average input power at reduced speeds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Least efficient load point driver or control input power  at 25% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Least efficient load point driver or control input power at 50% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Least efficient load point driver or control  input power at 75% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Least efficient load point driver or control input power at 100% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Least efficient load point weigted average input power at maximum rotating speed </t>
+  </si>
+  <si>
+    <t>Least efficient load point weighted average input power at reduced speeds</t>
+  </si>
+  <si>
+    <t>Most Efficient Pump Energy Index on nameplate</t>
+  </si>
+  <si>
+    <t>Least Efficient Pump Energy Index per HI 41.5</t>
+  </si>
+  <si>
+    <t>Rated (Most efficient) HI Energy Rating</t>
+  </si>
+  <si>
+    <t>Least efficient HI Energy Rating</t>
+  </si>
+  <si>
+    <t>Input the Rated (Most Efficient) control method used on the pump.
 Full speed
 Pressure control
 Temperature control
@@ -544,7 +548,7 @@
 Manual speed control</t>
   </si>
   <si>
-    <t>Input the most consumptive control method used on the pump.
+    <t>Input the least efficient control method used on the pump.
 Full speed
 Pressure control
 Temperature control
@@ -553,36 +557,28 @@
 Manual speed control</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Method I.
-Select Yes if pump uses full speed</t>
-  </si>
-  <si>
-    <t>I. Full Speed</t>
-  </si>
-  <si>
-    <t>CEI</t>
-  </si>
-  <si>
-    <t>Most Consumptive CEI</t>
-  </si>
-  <si>
-    <t>Least Consumptive CEI</t>
-  </si>
-  <si>
-    <t>Version 1.3</t>
-  </si>
-  <si>
-    <t>Brand name is displayed on the large label</t>
-  </si>
-  <si>
-    <t>Must be clearly listed on the permanently affixed pump nameplate.</t>
+    <t>If Pressure speed control is the rated (most efficient) control method, insert the control curve equation as function of flow rate(x) and head (y). For example y=mx+b or y=ax^2+bx+c, etc.</t>
+  </si>
+  <si>
+    <t>If Pressure speed control is the least efficient control method, insert the control curve equation as function of flow rate(x) and head(y). For example y=mx+b or y=ax^2+bx+c, etc.</t>
+  </si>
+  <si>
+    <t>Most Efficient CEI</t>
+  </si>
+  <si>
+    <t>Least Efficient CEI</t>
+  </si>
+  <si>
+    <t>Most Efficient ER</t>
+  </si>
+  <si>
+    <t>Least Efficient ER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1116,26 +1112,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1178,134 +1211,101 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1689,410 +1689,412 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" customWidth="1"/>
     <col min="14" max="16" width="30" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" customWidth="1"/>
+    <col min="17" max="17" width="28.109375" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" customWidth="1"/>
-    <col min="24" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="17.28515625" customWidth="1"/>
-    <col min="27" max="29" width="19.140625" customWidth="1"/>
-    <col min="30" max="30" width="12.140625" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" customWidth="1"/>
+    <col min="23" max="23" width="17.33203125" customWidth="1"/>
+    <col min="24" max="25" width="14.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" customWidth="1"/>
+    <col min="27" max="29" width="19.109375" customWidth="1"/>
+    <col min="30" max="30" width="12.109375" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" customWidth="1"/>
     <col min="32" max="32" width="14" customWidth="1"/>
-    <col min="33" max="34" width="14.7109375" customWidth="1"/>
-    <col min="35" max="35" width="20.28515625" customWidth="1"/>
-    <col min="36" max="36" width="18.28515625" customWidth="1"/>
-    <col min="37" max="38" width="17.85546875" customWidth="1"/>
-    <col min="39" max="1025" width="8.42578125" customWidth="1"/>
+    <col min="33" max="34" width="14.6640625" customWidth="1"/>
+    <col min="35" max="35" width="20.33203125" customWidth="1"/>
+    <col min="36" max="36" width="18.33203125" customWidth="1"/>
+    <col min="37" max="38" width="17.88671875" customWidth="1"/>
+    <col min="39" max="1025" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:39" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="62" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="63" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="4"/>
+      <c r="X1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63" t="s">
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="64" t="s">
+      <c r="AI1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM1" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" ht="35.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="64"/>
-      <c r="AA1" s="64"/>
-      <c r="AB1" s="54" t="s">
+      <c r="S2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="55" t="s">
+      <c r="T2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="1" t="s">
+      <c r="U2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="V2" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG2" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH2" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI2" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK2" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL2" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM2" s="13"/>
+    </row>
+    <row r="3" spans="1:39" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="R3" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="U3" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="W3" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="X3" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y3" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z3" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA3" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB3" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC3" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD3" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF3" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG3" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH3" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI3" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ3" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK3" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL3" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM3" s="13"/>
+    </row>
+    <row r="4" spans="1:39" ht="245.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="57"/>
+      <c r="B4" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="O4" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AM1" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="X2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="AG2" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH2" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI2" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="AJ2" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK2" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL2" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="31" t="s">
+      <c r="R4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="31" t="s">
+      <c r="W4" s="9"/>
+      <c r="X4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="33" t="s">
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="Y3" s="34" t="s">
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="Z3" s="34" t="s">
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI4" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ4" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="AA3" s="35" t="s">
+      <c r="AK4" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="AB3" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC3" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD3" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE3" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF3" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG3" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH3" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI3" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ3" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK3" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL3" s="43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" ht="245.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="M4" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="N4" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="O4" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="P4" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="R4" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="W4" s="57"/>
-      <c r="X4" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE4" s="60"/>
-      <c r="AF4" s="60"/>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI4" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ4" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK4" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL4" s="53" t="s">
-        <v>75</v>
-      </c>
+      <c r="AL4" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM4" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:Q2"/>
+    <mergeCell ref="AD4:AG4"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:AA1"/>
@@ -2102,7 +2104,8 @@
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="X4:AA4"/>
     <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2110,60 +2113,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="1025" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="3" max="1025" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Circulator Template and Export
</commit_message>
<xml_diff>
--- a/routes/er-circulator-listings.xlsx
+++ b/routes/er-circulator-listings.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hi-er\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E498C4B3-70EF-44FB-A4F7-C23F8BE79FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C99476-8277-42A5-ADE7-73783AADD710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5448" yWindow="3624" windowWidth="23040" windowHeight="12168" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6036" yWindow="1284" windowWidth="23040" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Lists" sheetId="2" r:id="rId2"/>
+    <sheet name="Choicelists" sheetId="2" r:id="rId2"/>
+    <sheet name="Version" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t>Pump Characteristics</t>
   </si>
@@ -474,9 +475,6 @@
   </si>
   <si>
     <t>Least Efficient Weighted Average Input Power</t>
-  </si>
-  <si>
-    <t>Version 1.4</t>
   </si>
   <si>
     <t>Rated (Most Efficient) Control Method</t>
@@ -574,12 +572,21 @@
   <si>
     <t>Least Efficient ER</t>
   </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Revision Date</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -609,6 +616,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1117,40 +1131,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1165,9 +1145,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1306,6 +1283,41 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1690,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM4"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AN2" sqref="AN2"/>
+      <selection activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1732,368 +1744,364 @@
     <col min="39" max="1025" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="4" t="s">
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="5" t="s">
+      <c r="W1" s="59"/>
+      <c r="X1" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="6" t="s">
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="7" t="s">
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="14" t="s">
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AI1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AK1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AK1" s="17" t="s">
+      <c r="AL1" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="AL1" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM1" s="19" t="s">
+    </row>
+    <row r="2" spans="1:38" ht="35.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI2" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL2" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="26" t="s">
         <v>67</v>
       </c>
+      <c r="O3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="R3" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="S3" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="T3" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="U3" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="V3" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="W3" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="X3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y3" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z3" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA3" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB3" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC3" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD3" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG3" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH3" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI3" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ3" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK3" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL3" s="43" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" ht="35.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="X2" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y2" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z2" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA2" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB2" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC2" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD2" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE2" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF2" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG2" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH2" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK2" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL2" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM2" s="13"/>
-    </row>
-    <row r="3" spans="1:39" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="O3" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="P3" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="R3" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="S3" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="T3" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="U3" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="V3" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="W3" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="X3" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y3" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z3" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA3" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB3" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC3" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD3" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE3" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF3" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG3" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH3" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI3" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ3" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK3" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL3" s="56" t="s">
+    <row r="4" spans="1:38" ht="245.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="AM3" s="13"/>
-    </row>
-    <row r="4" spans="1:39" ht="245.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="57"/>
-      <c r="B4" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="61" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="61" t="s">
+      <c r="O4" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="61" t="s">
+      <c r="P4" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="P4" s="62" t="s">
+      <c r="Q4" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="Q4" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="9" t="s">
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="W4" s="9"/>
-      <c r="X4" s="10" t="s">
+      <c r="W4" s="64"/>
+      <c r="X4" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="11" t="s">
+      <c r="Y4" s="65"/>
+      <c r="Z4" s="65"/>
+      <c r="AA4" s="65"/>
+      <c r="AB4" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="12" t="s">
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="64" t="s">
+      <c r="AE4" s="58"/>
+      <c r="AF4" s="58"/>
+      <c r="AG4" s="58"/>
+      <c r="AH4" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="AI4" s="65" t="s">
+      <c r="AI4" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="AJ4" s="65" t="s">
+      <c r="AJ4" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="AK4" s="66" t="s">
+      <c r="AK4" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AL4" s="66" t="s">
+      <c r="AL4" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="AM4" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:Q2"/>
     <mergeCell ref="AD4:AG4"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="V1:W1"/>
@@ -2104,20 +2112,42 @@
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="X4:AA4"/>
     <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B26E5A5A-C5AE-474D-9DC7-62CAB3182070}">
+          <x14:formula1>
+            <xm:f>Choicelists!$C$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>H5:M500</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{351A657C-50C2-4F90-BE3F-9DBA5BD5989E}">
+          <x14:formula1>
+            <xm:f>Choicelists!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>N5:O500</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{27B7D4B7-26A9-4F23-857D-42A5848ED29A}">
+          <x14:formula1>
+            <xm:f>Choicelists!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5:F500</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2128,44 +2158,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
+      <c r="A1" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2173,4 +2214,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712FBA03-4FCA-480E-9824-0D062368D4BA}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="54">
+        <v>45768</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>